<commit_message>
Attempted to build .exe package
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cevac\XDF-001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD22D9BB-52A9-46FE-95BC-0DAFE0A460EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876F6E9B-7ED2-4F00-9E75-8D13C9907CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{57CB118E-8278-42F0-84AE-CA474A92FF74}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>Item</t>
   </si>
@@ -116,21 +116,6 @@
     <t>A charger for lithium polymer batteries is the safest way to charge this type of battery.</t>
   </si>
   <si>
-    <t>Construction material, in this case it will be used for parts such as the wing ribs and stabilizers ribs</t>
-  </si>
-  <si>
-    <t>Construction material in this case for the spars that will reinforce critical areas such as the wing</t>
-  </si>
-  <si>
-    <t>1/16" x 4" x 36" Balsa Sheet</t>
-  </si>
-  <si>
-    <t>1/8" x 1/8" x 48" Balsa Strip/Stick</t>
-  </si>
-  <si>
-    <t>1/16 x 1/4 x 36 Balsa Strip</t>
-  </si>
-  <si>
     <t>ESP-32 Devkit 38 pins</t>
   </si>
   <si>
@@ -141,9 +126,6 @@
   </si>
   <si>
     <t>Source</t>
-  </si>
-  <si>
-    <t>Balsa USA</t>
   </si>
   <si>
     <t>electric propeller APC 11X7</t>
@@ -257,10 +239,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -601,7 +579,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,7 +609,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -639,7 +617,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -655,7 +633,7 @@
         <v>4.83</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G2">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -680,7 +658,7 @@
         <v>1.52</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G3">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -705,7 +683,7 @@
         <v>4.22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G4">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -730,7 +708,7 @@
         <v>2.58</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G5">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -755,7 +733,7 @@
         <v>0.7</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -780,7 +758,7 @@
         <v>2.14</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G7">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -789,7 +767,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -805,7 +783,7 @@
         <v>13.21</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G8">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -814,7 +792,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -830,7 +808,7 @@
         <v>15.5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G9">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -842,7 +820,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -855,7 +833,7 @@
         <v>2.74</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -864,7 +842,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
@@ -880,7 +858,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G11">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -905,7 +883,7 @@
         <v>0.99</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G12">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -917,7 +895,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -930,7 +908,7 @@
         <v>17.670000000000002</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G13">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -955,7 +933,7 @@
         <v>7.36</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G14">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -964,10 +942,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -980,7 +958,7 @@
         <v>22.99</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G15">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -989,10 +967,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
         <v>38</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1005,7 +983,7 @@
         <v>14.65</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G16">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -1014,10 +992,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1030,7 +1008,7 @@
         <v>18.989999999999998</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G17">
         <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
@@ -1038,79 +1016,16 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>5.01</v>
-      </c>
-      <c r="E18">
-        <f>Tabla1[[#This Row],[Quantity ]]*Tabla1[[#This Row],[Unit price]]</f>
-        <v>15.03</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18">
-        <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
-        <v>17.89</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19">
-        <v>1.25</v>
-      </c>
-      <c r="E19">
-        <f>Tabla1[[#This Row],[Quantity ]]*Tabla1[[#This Row],[Unit price]]</f>
-        <v>3.75</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19">
-        <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
-        <v>4.46</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>0.69</v>
-      </c>
-      <c r="E20">
-        <f>Tabla1[[#This Row],[Quantity ]]*Tabla1[[#This Row],[Unit price]]</f>
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20">
-        <f>ROUND(1.19*Tabla1[[#This Row],[Total Price]],2)</f>
-        <v>2.46</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="F20" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1125,19 +1040,16 @@
     <hyperlink ref="F11" r:id="rId9" display="URL very long, shorted" xr:uid="{B869D917-0BBF-4FA2-9C08-6AB07DCF7FB0}"/>
     <hyperlink ref="F12" r:id="rId10" display="URL very long, shorted" xr:uid="{6AF65191-9093-44CA-A434-65AC2B9E3853}"/>
     <hyperlink ref="F13" r:id="rId11" display="URL very long, shorted" xr:uid="{480648C1-D138-4172-A1F3-6B9257B81573}"/>
-    <hyperlink ref="F18" r:id="rId12" display="https://balsausa.com/products/1-16-x-4-x-36-balsa-sheet?_pos=1&amp;_sid=858eea6ce&amp;_ss=r" xr:uid="{E2AAB9D9-D621-4A62-ADE1-31A4682E63D2}"/>
-    <hyperlink ref="F19" r:id="rId13" display="https://balsausa.com/products/1-8-x-1-8-x-48-balsa-stick?_pos=1&amp;_sid=9f7ab279f&amp;_ss=r&amp;variant=47286589260066" xr:uid="{4C23825F-6A46-42B5-915F-EAB1BD1101F9}"/>
-    <hyperlink ref="F20" r:id="rId14" display="https://balsausa.com/collections/36-balsa-strips/products/1-16-x-1-4-x-36-balsa-stick" xr:uid="{FD4DFE9A-3E48-4ECD-957D-3332ED23A184}"/>
-    <hyperlink ref="F14" r:id="rId15" display="URL very long, shorted" xr:uid="{E64F23B2-F270-4375-AA9A-287B3C507512}"/>
-    <hyperlink ref="F9" r:id="rId16" display="aa" xr:uid="{FABE7EDF-7DDE-462D-A255-256D487D3E16}"/>
-    <hyperlink ref="F15" r:id="rId17" xr:uid="{26149171-8802-4F06-924C-935A7A889E39}"/>
-    <hyperlink ref="F16" r:id="rId18" xr:uid="{4F798240-33D7-42F9-B6A3-5B5B9D2B205C}"/>
-    <hyperlink ref="F17" r:id="rId19" xr:uid="{D7B157C8-755D-460E-BB17-513ED15287F9}"/>
+    <hyperlink ref="F14" r:id="rId12" display="URL very long, shorted" xr:uid="{E64F23B2-F270-4375-AA9A-287B3C507512}"/>
+    <hyperlink ref="F9" r:id="rId13" display="aa" xr:uid="{FABE7EDF-7DDE-462D-A255-256D487D3E16}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{26149171-8802-4F06-924C-935A7A889E39}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{4F798240-33D7-42F9-B6A3-5B5B9D2B205C}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{D7B157C8-755D-460E-BB17-513ED15287F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
   <tableParts count="1">
-    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>